<commit_message>
WhereWhenHowNoFoa_80, revised BKT controller, revised roll-up code
</commit_message>
<xml_diff>
--- a/Data/BKT_parameters.xlsx
+++ b/Data/BKT_parameters.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\AL\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB54107-6403-498A-8810-8F6282A2883E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D98DF41-302D-45AF-8AFA-8670386DAA4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21192" yWindow="708" windowWidth="24180" windowHeight="11868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First_revise" sheetId="1" r:id="rId1"/>
     <sheet name="Selection_as_step" sheetId="2" r:id="rId2"/>
-    <sheet name="each40" sheetId="3" r:id="rId3"/>
-    <sheet name="Human" sheetId="4" r:id="rId4"/>
+    <sheet name="Modular_40" sheetId="3" r:id="rId3"/>
+    <sheet name="WhereWhenHowNoFoa_80" sheetId="5" r:id="rId4"/>
+    <sheet name="Roney Patel" sheetId="4" r:id="rId5"/>
+    <sheet name="DS1706_Decision Tree" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="57">
   <si>
     <t>KC (ptype_selection)</t>
   </si>
@@ -188,6 +190,27 @@
   <si>
     <t>AL_40</t>
   </si>
+  <si>
+    <t>AS den5</t>
+  </si>
+  <si>
+    <t>M num3</t>
+  </si>
+  <si>
+    <t>M den3</t>
+  </si>
+  <si>
+    <t>M num4</t>
+  </si>
+  <si>
+    <t>AS den3</t>
+  </si>
+  <si>
+    <t>AS num3</t>
+  </si>
+  <si>
+    <t>AS num4</t>
+  </si>
 </sst>
 </file>
 
@@ -297,6 +320,421 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>WhereWhenHowNoFoa_80!$G$2:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.39180651620000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17724150929999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25534961490000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1179345731</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21611037250000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13101249179999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13386977380000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74101910090000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45076997880000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2486859243</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33251278560000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.36435982099999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.16554322099999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.2222223086</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>WhereWhenHowNoFoa_80!$J$2:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.26894416809999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14735349040000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15255836249999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20465841160000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27454436570000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8398643899999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1477222903</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3453968691</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.87328018139999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29136863680000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.45325456930000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.35908471110000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.23086939940000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.9511491999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F268-447A-815E-31A3A5F0A871}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="614539032"/>
+        <c:axId val="614535096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="614539032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="614535096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="614535096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="614539032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -377,7 +815,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Human!$A$2:$A$17</c:f>
+              <c:f>'Roney Patel'!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -433,7 +871,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Human!$C$2:$C$17</c:f>
+              <c:f>'Roney Patel'!$C$2:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -512,7 +950,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Human!$A$2:$A$17</c:f>
+              <c:f>'Roney Patel'!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -568,7 +1006,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Human!$I$2:$I$17</c:f>
+              <c:f>'Roney Patel'!$I$2:$I$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -832,7 +1270,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -927,7 +1365,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Human!$A$2:$A$17</c:f>
+              <c:f>'Roney Patel'!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -983,7 +1421,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Human!$D$2:$D$17</c:f>
+              <c:f>'Roney Patel'!$D$2:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1062,7 +1500,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Human!$A$2:$A$17</c:f>
+              <c:f>'Roney Patel'!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -1118,7 +1556,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Human!$J$2:$J$17</c:f>
+              <c:f>'Roney Patel'!$J$2:$J$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1382,7 +1820,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1476,7 +1914,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Human!$A$2:$A$17</c:f>
+              <c:f>'Roney Patel'!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -1532,7 +1970,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Human!$E$2:$E$17</c:f>
+              <c:f>'Roney Patel'!$E$2:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1611,7 +2049,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Human!$A$2:$A$17</c:f>
+              <c:f>'Roney Patel'!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -1667,7 +2105,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Human!$K$2:$K$17</c:f>
+              <c:f>'Roney Patel'!$K$2:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1933,7 +2371,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2027,7 +2465,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Human!$A$2:$A$17</c:f>
+              <c:f>'Roney Patel'!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -2083,7 +2521,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Human!$F$2:$F$17</c:f>
+              <c:f>'Roney Patel'!$F$2:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2162,7 +2600,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Human!$A$2:$A$17</c:f>
+              <c:f>'Roney Patel'!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -2218,7 +2656,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Human!$L$2:$L$17</c:f>
+              <c:f>'Roney Patel'!$L$2:$L$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2484,6 +2922,920 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Roney Patel'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Learn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Roney Patel'!$D$2:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.26894416809999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14735349040000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15255836249999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20465841160000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27454436570000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8398643899999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1477222903</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3453968691</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.87328018139999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29136863680000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.45325456930000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36245830690000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.35908471110000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.23086939940000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.9511491999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.27714751970000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2841594636375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Roney Patel'!$J$2:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.2639624954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1994582825</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3013751348</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15959680370000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24869410280000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1613566193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12017980390000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81309677250000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47817773050000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29957131259999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.32414618680000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0825429E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.41356532579999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.229096997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26699057859999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8909449999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26756498647499999</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>0.2841594636375</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>0.26756498647499999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6F10-42DB-A65F-15B04571B333}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="670083664"/>
+        <c:axId val="670084320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="670083664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="670084320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="670084320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="670083664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Roney Patel'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Known</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Roney Patel'!$C$2:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.6141394443</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26268298039999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37928708220000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34221579050000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59731719179999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81046531509999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68147751369999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69774662320000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.82299883350000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90589735270000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.51863176460000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.67702156889999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93918918380000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.78648461260000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85897010060000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.39563202409999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.64313483637500013</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Roney Patel'!$I$2:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.15527868140000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5584101999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3594E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4184E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9874300000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0397632000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5084340000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5429999999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25392906910000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.862E-7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3000000000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1078957988</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5219100000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0998200000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.72314782E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.6177577599999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.30457688625E-2</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>0.64313483637500013</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>4.30457688625E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E497-4C4C-91B7-396C07A757E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="713133568"/>
+        <c:axId val="713136520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="713133568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="713136520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="713136520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="713133568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2644,8 +3996,128 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2672,8 +4144,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2774,7 +4246,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2806,10 +4278,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3130,6 +4602,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4664,7 +6147,1585 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>659130</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>339090</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FC1090E-257F-4C77-B632-958D0E726FB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4810,6 +7871,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>293370</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>224790</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B67EB7FD-3752-41FE-9321-397040633674}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>186690</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>118110</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFDE0275-9447-46FB-B210-A4B13751ABEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5523,9 +8656,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" activeCellId="1" sqref="A10:E10 A15:E18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6061,9 +9192,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:E25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6503,11 +9632,751 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F6639C-CB69-4962-AC0D-208D5AAE04C3}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.29534158729999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.39180651620000001</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.1292214813</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7.4738000000000003E-6</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.39180651620000001</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.6141394443</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.26894416809999999</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L2" s="1">
+        <v>5.3997131300000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>9.2500000000000001E-8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.17724150929999999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.1154442933</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.7200335E-3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.17724150929999999</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.26268298039999999</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.14735349040000001</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.14169207480000001</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.10603757329999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.25534961490000002</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.18390776480000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.7058157000000002E-3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.25534961490000002</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.37928708220000001</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.15255836249999999</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.2912968675</v>
+      </c>
+      <c r="L4" s="1">
+        <v>7.3293134800000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.1179345731</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.17028673850000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.64054756E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.1179345731</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.34221579050000001</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.20465841160000001</v>
+      </c>
+      <c r="K5" s="1">
+        <v>7.9566106600000006E-2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.1056923476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.21611037250000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.22659976309999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4.6512085000000002E-3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.21611037250000001</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.59731719179999998</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.27454436570000001</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L6" s="1">
+        <v>3.0432322099999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4.9399999999999999E-8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.13101249179999999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.10251977600000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.1093334243</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.13101249179999999</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.81046531509999997</v>
+      </c>
+      <c r="J7" s="1">
+        <v>9.8398643899999999E-2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>6.0955775900000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.966E-7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.13386977380000001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7.6005394000000004E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.17294744440000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.13386977380000001</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.68147751369999998</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.1477222903</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>7.6830645200000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.74101910090000001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3.1308002000000001E-3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8.7044513399999995E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.74101910090000001</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.69774662320000003</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.3453968691</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1.79947209E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.0394408200000002E-2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.45076997880000003</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.28543795970000002</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5.8500779999999997E-4</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.45076997880000003</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.82299883350000003</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.87328018139999997</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L10" s="1">
+        <v>3.9493615599999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.24703025679999999</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4.4744860000000002E-4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.2486859243</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.90589735270000005</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.29136863680000002</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L11" s="1">
+        <v>6.1083600199999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.34976221190000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.8961795E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.33251278560000003</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.51863176460000004</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.45325456930000002</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.25210989950000001</v>
+      </c>
+      <c r="L12" s="1">
+        <v>3.6401996700000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.29875630850000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.4868750000000002E-4</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.67702156889999998</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2.4632637499999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.3565853289</v>
+      </c>
+      <c r="C14" s="1">
+        <v>8.678987E-4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.36435982099999997</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.93918918380000005</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.35908471110000001</v>
+      </c>
+      <c r="K14" s="1">
+        <v>9.9270009999999995E-3</v>
+      </c>
+      <c r="L14" s="1">
+        <v>3.2769833499999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.963E-7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.2486859243</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.1792279272</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5.1213167099999998E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.16554322099999999</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.78648461260000002</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.23086939940000001</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2.6333594799999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.7023049999999997E-4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.33251278560000003</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.21552729540000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.1364855053</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.2222223086</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.85897010060000001</v>
+      </c>
+      <c r="J16" s="1">
+        <v>5.9511491999999999E-2</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L16" s="1">
+        <v>5.2998410400000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4.4014400000000003E-5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.39563202409999998</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1.85243826E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.36435982099999997</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.2112306531</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2.3975899999999999E-5</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.30060474469999998</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.2333870000000001E-3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.3358233806</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2.1272344000000001E-3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.30966592259999998</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.0595144E-3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.4695761678</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.6173798E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.16554322099999999</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.21353625800000001</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.3049450400000001E-2</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.2222223086</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.18053486399999999</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1.72232059E-2</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.1062568577</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2.1089374000000001E-3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC64782-EA15-40EF-A234-BD6824549EFA}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7223,4 +11092,582 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B3F4C0-C98E-4722-8F55-868E057DAC2A}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.19355408E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.54074286760000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.15284457900000001</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.24849261E-2</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.4199999999999996E-8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.29699766119999998</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4.6514946600000003E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4.7557043600000001E-2</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3E-10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.32853728030000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.6815718000000001E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.5819209099999999E-2</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2E-8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.19986238789999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.8546999999999997E-6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.99999614530000003</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.3922400000000001E-5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.7473589599999998E-2</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.5629000000000001E-6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.26105822480000002</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.2229948699999998E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6.2751969399999996E-2</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.044E-7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.33093849079999998</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3.7066300000000003E-4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3.7375157899999997E-2</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.89473858019999997</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.8343147E-3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>6.3767564799999996E-2</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.1700000000000002E-6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.99998596529999995</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.47164242200000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.6173798E-3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.43474860510000002</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.6173798E-3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.6942514000000001E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6.1018388799999997E-2</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.47503412309999998</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.6173798E-3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.28814E-5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.45131995920000001</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>8.4562183000000003E-3</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2.7999999999999998E-9</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.75275907929999997</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.9827059999999999E-3</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5.3892976299999999E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8.266177E-4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>6.1498143200000001E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>8.5717021500000004E-2</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.4708804694</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.57171321119999996</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.32640982410000002</v>
+      </c>
+      <c r="D18" s="1">
+        <v>9.5342460000000001E-4</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.37402518550000002</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.0481533999999999E-3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.2723347E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.40375444910000002</v>
+      </c>
+      <c r="D20" s="1">
+        <v>6.9330369999999995E-4</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1">
+        <v>6.4451339000000003E-3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.14163582329999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6.5370163000000002E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.52388010139999996</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.35067242339999999</v>
+      </c>
+      <c r="D23" s="1">
+        <v>8.6814960000000001E-4</v>
+      </c>
+      <c r="E23" s="1">
+        <v>8.1078044399999993E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2.25098561E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
+    <sortCondition ref="A1:A23"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>